<commit_message>
Add hike 8 & 9
</commit_message>
<xml_diff>
--- a/data/52-Hike-Challenge-Hiking-Log_2020.xlsx
+++ b/data/52-Hike-Challenge-Hiking-Log_2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebciii3/Documents/Personal/Travel/Trails/Hike Notes and Tracking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebciii3/Documents/Computer Stuff/R Projects/52_saunters_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206AB3C5-BC0E-9C42-AD73-ABCABBC1A6D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B6D4DB-9D87-324B-8AE3-517DA703B7ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="460" windowWidth="23700" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="159">
   <si>
     <t>Hike #</t>
   </si>
@@ -492,6 +492,15 @@
   </si>
   <si>
     <t xml:space="preserve">               52 Weekly Sauntering Challenge Log 2020</t>
+  </si>
+  <si>
+    <t>Skyline&gt;Fireline from Hickory Run</t>
+  </si>
+  <si>
+    <t>Nolde Forest SP</t>
+  </si>
+  <si>
+    <t>Nolde Forest Trail</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1064,7 @@
       <pane xSplit="8" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1349,27 +1358,59 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="1"/>
+      <c r="B14" s="13">
+        <v>43864</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="15">
+        <v>6.7</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.1361111111111111</v>
+      </c>
+      <c r="G14" s="15">
+        <v>850</v>
+      </c>
+      <c r="H14" s="15">
+        <v>4</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="1"/>
+      <c r="B15" s="13">
+        <v>43869</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" s="15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F15" s="28">
+        <v>9.375E-2</v>
+      </c>
+      <c r="G15" s="15">
+        <v>653</v>
+      </c>
+      <c r="H15" s="15">
+        <v>4</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1950,12 +1991,12 @@
       <c r="D60" s="18"/>
       <c r="E60" s="19">
         <f>SUM(E7:E59)</f>
-        <v>25.599999999999998</v>
+        <v>36.4</v>
       </c>
       <c r="F60" s="19"/>
       <c r="G60" s="19">
         <f>SUM(G7:G59)</f>
-        <v>2876</v>
+        <v>4379</v>
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="7"/>

</xml_diff>